<commit_message>
Unittests fuer Methode insert_anzahl_kinder_an_pv_beitrag geschrieben.
</commit_message>
<xml_diff>
--- a/src/main/insert Sozialversicherungsdaten/5 Anzahl Kinder Arbeitnehmer PV-Beitrag.xlsx
+++ b/src/main/insert Sozialversicherungsdaten/5 Anzahl Kinder Arbeitnehmer PV-Beitrag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert Sozialversicherungsdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D17F04C-681A-4F6A-8604-11C4F7FD20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BD1E0A-91C5-425A-92F5-573A431E419F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4992" yWindow="1728" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>